<commit_message>
test: Improves the precision of test_get_sharepoint_data()
Checks that the output of AgingReport.get_sharepoint_data() equals the 
input data for test_populate_report()
</commit_message>
<xml_diff>
--- a/app/tests/integration_tests/aging_report/SampleAgingReport.xlsx
+++ b/app/tests/integration_tests/aging_report/SampleAgingReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdaly/Documents/PyProjects/py3.7.7/DGS/priority-vendor-aging-report/app/tests/integration_tests/aging_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77C649C-5734-2649-945E-23E554ABB811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679951EA-C88E-BE4A-ADA2-D7FD492A52B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{C04EB209-85D3-8645-AAEE-849A20F8963C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>EST#</t>
   </si>
@@ -68,27 +68,6 @@
   </si>
   <si>
     <t>Disney</t>
-  </si>
-  <si>
-    <t>201111-R</t>
-  </si>
-  <si>
-    <t>202222-R</t>
-  </si>
-  <si>
-    <t>203333-R</t>
-  </si>
-  <si>
-    <t>204444-R</t>
-  </si>
-  <si>
-    <t>101111-R</t>
-  </si>
-  <si>
-    <t>102222-R</t>
-  </si>
-  <si>
-    <t>103333-R</t>
   </si>
   <si>
     <t>Invoice#3</t>
@@ -507,7 +486,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,13 +525,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>101</v>
       </c>
       <c r="D2" s="4">
         <v>44013</v>
@@ -570,18 +549,18 @@
         <v>966</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>102</v>
       </c>
       <c r="D3" s="4">
         <v>44013</v>
@@ -599,18 +578,18 @@
         <v>960</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="3">
+        <v>103</v>
       </c>
       <c r="D4" s="4">
         <v>44834</v>
@@ -628,18 +607,18 @@
         <v>923</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>201</v>
       </c>
       <c r="D5" s="4">
         <v>44104</v>
@@ -657,18 +636,18 @@
         <v>903</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>202</v>
       </c>
       <c r="D6" s="4">
         <v>44013</v>
@@ -686,18 +665,18 @@
         <v>903</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="3">
+        <v>203</v>
       </c>
       <c r="D7" s="4">
         <v>44044</v>
@@ -715,18 +694,18 @@
         <v>888</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="3">
+        <v>204</v>
       </c>
       <c r="D8" s="4">
         <v>44834</v>
@@ -744,7 +723,7 @@
         <v>851</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: Ensures Invoice Number and EST# are read as strings
Previously the Invoice Number and EST# could be read in as int64 if none 
of the rows had strings. This commit forces the type to string
</commit_message>
<xml_diff>
--- a/app/tests/integration_tests/aging_report/SampleAgingReport.xlsx
+++ b/app/tests/integration_tests/aging_report/SampleAgingReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdaly/Documents/PyProjects/py3.7.7/DGS/priority-vendor-aging-report/app/tests/integration_tests/aging_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679951EA-C88E-BE4A-ADA2-D7FD492A52B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840C9867-FE3B-B349-A877-173D9B6724E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{C04EB209-85D3-8645-AAEE-849A20F8963C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>EST#</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>#4</t>
-  </si>
-  <si>
-    <t>#5</t>
   </si>
   <si>
     <t>P111:1</t>
@@ -483,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC5109F-C98C-A24E-8D08-53370E9D6C9C}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +546,7 @@
         <v>966</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -578,7 +575,7 @@
         <v>960</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -607,7 +604,7 @@
         <v>923</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -636,7 +633,7 @@
         <v>903</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -665,7 +662,7 @@
         <v>903</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -694,15 +691,15 @@
         <v>888</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5</v>
       </c>
       <c r="C8" s="3">
         <v>204</v>
@@ -723,7 +720,7 @@
         <v>851</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -816,15 +813,6 @@
       <c r="F18" s="3"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Implement `AgingReport.populate_report()` (#123)
* test: Improves the precision of test_get_sharepoint_data()
Checks that the output of AgingReport.get_sharepoint_data() equals the 
input data for test_populate_report()

* feat: Implements AgingReport.populate_report()

* fix: Ensures Invoice Number and EST# are read as strings
Previously the Invoice Number and EST# could be read in as int64 if none 
of the rows had strings. This commit forces the type to string

* ci: Bump black and typer to fix failing tox tests
For more information, reference this github issue: 
https://github.com/tiangolo/typer/issues/377

* refactor: Uses EST# to match invoices to citibuy and renames column
Instead of using the Vendor ID and Invoice Number to match, this commit 
uses EST# and renames the column Invoice Key to make it clearer
</commit_message>
<xml_diff>
--- a/app/tests/integration_tests/aging_report/SampleAgingReport.xlsx
+++ b/app/tests/integration_tests/aging_report/SampleAgingReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamdaly/Documents/PyProjects/py3.7.7/DGS/priority-vendor-aging-report/app/tests/integration_tests/aging_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77C649C-5734-2649-945E-23E554ABB811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840C9867-FE3B-B349-A877-173D9B6724E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{C04EB209-85D3-8645-AAEE-849A20F8963C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>EST#</t>
   </si>
@@ -70,27 +70,6 @@
     <t>Disney</t>
   </si>
   <si>
-    <t>201111-R</t>
-  </si>
-  <si>
-    <t>202222-R</t>
-  </si>
-  <si>
-    <t>203333-R</t>
-  </si>
-  <si>
-    <t>204444-R</t>
-  </si>
-  <si>
-    <t>101111-R</t>
-  </si>
-  <si>
-    <t>102222-R</t>
-  </si>
-  <si>
-    <t>103333-R</t>
-  </si>
-  <si>
     <t>Invoice#3</t>
   </si>
   <si>
@@ -107,9 +86,6 @@
   </si>
   <si>
     <t>#4</t>
-  </si>
-  <si>
-    <t>#5</t>
   </si>
   <si>
     <t>P111:1</t>
@@ -504,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC5109F-C98C-A24E-8D08-53370E9D6C9C}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,13 +522,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>101</v>
       </c>
       <c r="D2" s="4">
         <v>44013</v>
@@ -570,18 +546,18 @@
         <v>966</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>102</v>
       </c>
       <c r="D3" s="4">
         <v>44013</v>
@@ -599,18 +575,18 @@
         <v>960</v>
       </c>
       <c r="I3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="3">
+        <v>103</v>
       </c>
       <c r="D4" s="4">
         <v>44834</v>
@@ -628,18 +604,18 @@
         <v>923</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>201</v>
       </c>
       <c r="D5" s="4">
         <v>44104</v>
@@ -657,18 +633,18 @@
         <v>903</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>202</v>
       </c>
       <c r="D6" s="4">
         <v>44013</v>
@@ -686,18 +662,18 @@
         <v>903</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="3">
+        <v>203</v>
       </c>
       <c r="D7" s="4">
         <v>44044</v>
@@ -715,18 +691,18 @@
         <v>888</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>204</v>
       </c>
       <c r="D8" s="4">
         <v>44834</v>
@@ -744,7 +720,7 @@
         <v>851</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -837,15 +813,6 @@
       <c r="F18" s="3"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>